<commit_message>
updated lat lon outputs for TT rule + updated scripts for TRI facilities that dont drop facilities
</commit_message>
<xml_diff>
--- a/data/hfc_facilities-4-8-22_w_additions V2_frsID_updatedlatlon.xlsx
+++ b/data/hfc_facilities-4-8-22_w_additions V2_frsID_updatedlatlon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\Git Repos\F_Gas_Rules\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB736A80-97B9-430B-95FC-2AB6C32A51A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFED859-200D-4310-B7A7-AC481537A46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B999005D-378C-4D50-B09E-E8C4AF2F8FB6}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{B999005D-378C-4D50-B09E-E8C4AF2F8FB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -801,31 +801,31 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -878,7 +878,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -925,7 +925,7 @@
         <v>325120</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -960,7 +960,7 @@
         <v>110000514122</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>325311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>41.637813999999999</v>
       </c>
       <c r="E5">
-        <v>87.463561999999996</v>
+        <v>-87.463561999999996</v>
       </c>
       <c r="F5" t="s">
         <v>85</v>
@@ -1060,7 +1060,7 @@
         <v>325120</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>325120</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>110000599479</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>325120</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1209,8 +1209,7 @@
         <v>38.29562</v>
       </c>
       <c r="E9">
-        <f>--81.464326</f>
-        <v>81.464326</v>
+        <v>-81.464326</v>
       </c>
       <c r="F9" t="s">
         <v>89</v>
@@ -1231,7 +1230,7 @@
         <v>110069506877</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>22</v>
       </c>
@@ -1272,7 +1271,7 @@
       </c>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
@@ -1308,7 +1307,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -1349,7 +1348,7 @@
       </c>
       <c r="Q12" s="7"/>
     </row>
-    <row r="13" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1385,7 +1384,7 @@
         <v>110008381438</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>44</v>
       </c>
@@ -1432,7 +1431,7 @@
         <v>325120</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>44</v>
       </c>
@@ -1480,60 +1479,60 @@
         <v>325120</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
       <c r="E18" s="30"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" s="31"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C24" s="31"/>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C27" s="32"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C28" s="6"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C29" s="6"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C30" s="18"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C31" s="19"/>
       <c r="D31" s="33"/>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C32" s="19"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>

</xml_diff>